<commit_message>
xlsx mit constraints ergänzt
</commit_message>
<xml_diff>
--- a/doc/LG_GeolAssetsCatalogues_V2_220328.xlsx
+++ b/doc/LG_GeolAssetsCatalogues_V2_220328.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836" firstSheet="3" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7060" tabRatio="836" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,6 @@
     <sheet name="StatusAssetUseItem" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="760">
   <si>
     <t>Wertekataloge für das Datenmodell GeolAssets und dessen Erweiterung LG_GeolAssets für die Landesgeologie</t>
   </si>
@@ -2342,6 +2341,21 @@
   </si>
   <si>
     <t>Special scientific interest</t>
+  </si>
+  <si>
+    <t>Wenn das Asset nicht von nationaler Relevanz ist, muss dein Typ definiert werden</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE NOT(IsNatRel): NOT (DEFINED (TypeNatRel));</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE (IsNatRel): DEFINED(TypeNatRel);</t>
+  </si>
+  <si>
+    <t>SET CONSTRAINT WHERE AssetItemPart-&gt;IsExtract: DEFINED (AssetItemMain);</t>
+  </si>
+  <si>
+    <t>Jedes AssetPart, dass ein Extract ist, muss ein Main besitzen</t>
   </si>
 </sst>
 </file>
@@ -4969,7 +4983,7 @@
   </sheetPr>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -5473,10 +5487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5821,33 +5835,28 @@
         <v>596</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="25" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>660</v>
+      <c r="B13" s="21" t="s">
+        <v>7</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>662</v>
+        <v>634</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>661</v>
+        <v>759</v>
       </c>
       <c r="F13" s="20" t="s">
-        <v>663</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>645</v>
-      </c>
-      <c r="O13" s="17" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="50" x14ac:dyDescent="0.35">
+        <v>758</v>
+      </c>
+      <c r="O13" s="17"/>
+    </row>
+    <row r="14" spans="1:15" ht="26" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5861,20 +5870,19 @@
         <v>662</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="F14" s="20" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H14" s="14"/>
       <c r="O14" s="17" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="50" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5888,17 +5896,17 @@
         <v>662</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="14"/>
       <c r="O15" s="17" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
@@ -5915,135 +5923,201 @@
         <v>662</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>645</v>
       </c>
       <c r="H16" s="13"/>
       <c r="O16" s="17" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="17" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>669</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>645</v>
+      </c>
       <c r="H17" s="13"/>
       <c r="O17" s="17" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="18" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>756</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>645</v>
+      </c>
       <c r="H18" s="13"/>
       <c r="O18" s="17" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="19" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>660</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>755</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>757</v>
+      </c>
       <c r="H19" s="13"/>
       <c r="O19" s="17" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="20" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H20" s="13"/>
       <c r="O20" s="17" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="21" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H21" s="13"/>
       <c r="O21" s="17" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="22" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H22" s="13"/>
       <c r="O22" s="17" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="23" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H23" s="13"/>
       <c r="O23" s="17" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="24" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H24" s="13"/>
       <c r="O24" s="17" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="25" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H25" s="13"/>
       <c r="O25" s="17" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="26" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
       <c r="H26" s="13"/>
       <c r="O26" s="17" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H27" s="13"/>
+      <c r="O27" s="17" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="27" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H27" s="13"/>
-      <c r="O27" s="12"/>
-    </row>
-    <row r="28" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H28" s="13"/>
       <c r="O28" s="12"/>
     </row>
-    <row r="29" spans="8:15" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H29" s="13"/>
-      <c r="O29" s="17" t="s">
+      <c r="O29" s="12"/>
+    </row>
+    <row r="30" spans="1:15" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="H30" s="13"/>
+      <c r="O30" s="17" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="30" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H30" s="13"/>
-      <c r="O30" s="12" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="31" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H31" s="13"/>
       <c r="O31" s="12" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H32" s="13"/>
+      <c r="O32" s="12" t="s">
         <v>596</v>
-      </c>
-    </row>
-    <row r="32" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="O32" s="12" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="33" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O33" s="12" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34" s="12" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O34" s="12"/>
-    </row>
     <row r="35" spans="15:15" x14ac:dyDescent="0.25">
-      <c r="O35" s="12" t="s">
-        <v>613</v>
-      </c>
+      <c r="O35" s="12"/>
     </row>
     <row r="36" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O36" s="12" t="s">
-        <v>596</v>
+        <v>613</v>
       </c>
     </row>
     <row r="37" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O37" s="12" t="s">
-        <v>614</v>
+        <v>596</v>
       </c>
     </row>
     <row r="38" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O38" s="12" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="39" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O39" s="12" t="s">
         <v>615</v>
       </c>
     </row>

</xml_diff>